<commit_message>
Temporary commit: adds distributed solar policy proxy, land-use regulation, RPS (to meet RED targets), and boiler shifting
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BDESC/BAU Distributed Electricity Source Capacities.xlsx
+++ b/InputData/bldgs/BDESC/BAU Distributed Electricity Source Capacities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://artelys778.sharepoint.com/sites/Agora-EPStool-Artelys/Documents partages/Artelys/3 - Livrables/1. all data/2. A checker par Paul/Uploaded/10. BAU Distributed Electricity Quantities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\bldgs\BDESC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="8_{C56910BB-A762-4B0B-AC8D-940FC4AECB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3966E3D4-8957-4197-AAFD-CB43D06A4772}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E7923C-9888-4571-BA42-DAB3CDA62BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" xr2:uid="{018189C1-0CD4-4228-8640-AB6E9BB2D151}"/>
+    <workbookView xWindow="30510" yWindow="1710" windowWidth="24555" windowHeight="15300" xr2:uid="{018189C1-0CD4-4228-8640-AB6E9BB2D151}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
   <si>
     <t>BDEQ BAU Distributed Electricity Source Capacity</t>
   </si>
@@ -279,16 +279,38 @@
   <si>
     <t>hydrogen combined cycle</t>
   </si>
+  <si>
+    <t>Home rooftop</t>
+  </si>
+  <si>
+    <t>Commercial &amp; Industrial rooftop</t>
+  </si>
+  <si>
+    <t>home rooftop</t>
+  </si>
+  <si>
+    <t>commercial &amp; industrial rooftop</t>
+  </si>
+  <si>
+    <t>Split between home &amp; commercial rooftops</t>
+  </si>
+  <si>
+    <t>Solar Power europe: EU Rooftop Solar Standard alone could solar power 56 million homes</t>
+  </si>
+  <si>
+    <t>https://www.solarpowereurope.org/press-releases/eu-rooftop-solar-standard-alone-could-solar-power-56-million-homes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1067,7 +1089,7 @@
     <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1113,6 +1135,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="36" applyFill="1"/>
+    <xf numFmtId="168" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="55">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1195,7 +1220,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1263650</xdr:colOff>
+      <xdr:colOff>1266825</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>78641</xdr:rowOff>
     </xdr:to>
@@ -1245,7 +1270,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>410170</xdr:colOff>
+      <xdr:colOff>406995</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>78105</xdr:rowOff>
     </xdr:to>
@@ -1301,9 +1326,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1341,7 +1366,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1447,7 +1472,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1589,7 +1614,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1597,28 +1622,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C8B6E5-3AAE-4BB5-A9E2-A69A34ECA6F1}">
-  <dimension ref="B10:D21"/>
+  <dimension ref="B10:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" style="1"/>
+    <col min="1" max="2" width="10.81640625" style="1"/>
     <col min="3" max="3" width="44" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.85546875" style="1"/>
+    <col min="4" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
@@ -1629,7 +1654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
@@ -1637,7 +1662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
@@ -1645,7 +1670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1653,23 +1678,34 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="2" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="38"/>
-    </row>
-    <row r="20" spans="2:4" ht="15">
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="2:4" ht="15">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="38"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1678,48 +1714,49 @@
     <hyperlink ref="D13" r:id="rId1" display="Source : Solar Power europe : Global Market Outlook 2023-2027, figure 21.1" xr:uid="{970C4275-1DF1-4C9C-8780-AC7E2338970A}"/>
     <hyperlink ref="D14" r:id="rId2" xr:uid="{89C2EB55-9D18-4EB5-86FB-F0E1711AB597}"/>
     <hyperlink ref="D15" r:id="rId3" display="ENTSOE Statistical Factsheets 2018, 2021 and 2022" xr:uid="{B6CEE78D-E37F-4107-8CF7-EA8199B6453F}"/>
+    <hyperlink ref="D17" r:id="rId4" xr:uid="{DF4A4DBC-A58B-4B49-AD50-B6F951953422}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32680363-802D-49C5-A324-7CE370994BC0}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B26" sqref="B26:J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
@@ -1757,7 +1794,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1797,7 +1834,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1837,554 +1874,706 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="8" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9">
+        <v>68.8</v>
+      </c>
+      <c r="C9" s="45">
+        <f>B9/SUM(B9:B10)</f>
+        <v>0.39631336405529954</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10">
+        <v>104.8</v>
+      </c>
+      <c r="C10" s="45">
+        <f>B10/SUM(B9:B10)</f>
+        <v>0.60368663594470051</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="43"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="8"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="9" t="s">
+      <c r="B13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="9"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="9" t="s">
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="9"/>
-    </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1">
-      <c r="A13" s="7" t="s">
+      <c r="B15" s="9"/>
+    </row>
+    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="12" t="s">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B18" s="13">
         <v>2020</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C18" s="13">
         <v>2021</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D18" s="13">
         <v>2022</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E18" s="14">
         <v>2025</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F18" s="14">
         <v>2030</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G18" s="14">
         <v>2035</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H18" s="14">
         <v>2040</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I18" s="14">
         <v>2045</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J18" s="15">
         <v>2050</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="18" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B15">
+      <c r="B19">
         <v>136620</v>
       </c>
-      <c r="C15">
+      <c r="C19">
         <v>162354</v>
       </c>
-      <c r="D15">
+      <c r="D19">
         <v>198326</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E19" s="19">
         <v>253217</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F19" s="19">
         <v>344702</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G19" s="19">
         <v>436187</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H19" s="19">
         <v>527672</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I19" s="19">
         <v>619157</v>
       </c>
-      <c r="J15" s="20">
+      <c r="J19" s="20">
         <v>710642</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="18" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B16">
+      <c r="B20">
         <v>2321</v>
       </c>
-      <c r="C16">
+      <c r="C20">
         <v>2321</v>
       </c>
-      <c r="D16">
+      <c r="D20">
         <v>2321</v>
       </c>
-      <c r="E16">
+      <c r="E20">
         <v>2321</v>
       </c>
-      <c r="F16">
+      <c r="F20">
         <v>2321</v>
       </c>
-      <c r="G16">
+      <c r="G20">
         <v>2321</v>
       </c>
-      <c r="H16">
+      <c r="H20">
         <v>2321</v>
       </c>
-      <c r="I16">
+      <c r="I20">
         <v>2321</v>
       </c>
-      <c r="J16" s="29">
+      <c r="J20" s="29">
         <v>2321</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="18" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B17">
-        <f>B15+B16</f>
+      <c r="B21">
+        <f>B19+B20</f>
         <v>138941</v>
       </c>
-      <c r="C17">
+      <c r="C21">
         <v>164675</v>
       </c>
-      <c r="D17">
+      <c r="D21">
         <v>200647</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E21" s="19">
         <v>255538</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F21" s="19">
         <v>347023</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G21" s="19">
         <v>438508</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H21" s="19">
         <v>529993</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I21" s="19">
         <v>621478</v>
       </c>
-      <c r="J17" s="20">
+      <c r="J21" s="20">
         <v>712963</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="18" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B18">
+      <c r="B22">
         <v>14542</v>
       </c>
-      <c r="C18">
+      <c r="C22">
         <v>15137</v>
       </c>
-      <c r="D18">
+      <c r="D22">
         <v>16749</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E22" s="19">
         <v>24120</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F22" s="19">
         <v>36405</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G22" s="19">
         <v>48690</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H22" s="19">
         <v>60975</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I22" s="19">
         <v>73260</v>
       </c>
-      <c r="J18" s="20">
+      <c r="J22" s="20">
         <v>85545</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1">
-      <c r="A19" s="16" t="s">
+    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B23" s="17">
         <v>162590</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C23" s="17">
         <v>173316</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D23" s="17">
         <v>187373</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E23" s="22">
         <v>209765</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F23" s="22">
         <v>247085</v>
       </c>
-      <c r="G19" s="22">
+      <c r="G23" s="22">
         <v>284405</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H23" s="22">
         <v>321725</v>
       </c>
-      <c r="I19" s="22">
+      <c r="I23" s="22">
         <v>359045</v>
       </c>
-      <c r="J19" s="23">
+      <c r="J23" s="23">
         <v>396365</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="7" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B20">
-        <f>B15*B6</f>
+      <c r="B24">
+        <f>B19*B6</f>
         <v>46450.8</v>
       </c>
-      <c r="C20">
-        <f>$C$15*C6</f>
+      <c r="C24">
+        <f>$C$19*C6</f>
         <v>55200.36</v>
       </c>
-      <c r="D20">
-        <f>$D$15*D6</f>
+      <c r="D24">
+        <f>$D$19*D6</f>
         <v>67430.840000000011</v>
       </c>
-      <c r="E20">
-        <f>$E$15*G6</f>
+      <c r="E24">
+        <f>$E$19*G6</f>
         <v>99387.672499999986</v>
       </c>
-      <c r="F20">
-        <f>$F$15*I6</f>
+      <c r="F24">
+        <f>$F$19*I6</f>
         <v>141327.81999999998</v>
       </c>
-      <c r="G20">
-        <f>$G$15*J6</f>
+      <c r="G24">
+        <f>$G$19*J6</f>
         <v>178836.66999999998</v>
       </c>
-      <c r="H20">
-        <f>$H$15*K6</f>
+      <c r="H24">
+        <f>$H$19*K6</f>
         <v>216345.52</v>
       </c>
-      <c r="I20">
-        <f>$I$15*L6</f>
+      <c r="I24">
+        <f>$I$19*L6</f>
         <v>253854.37</v>
       </c>
-      <c r="J20">
-        <f>$J$15*L6</f>
+      <c r="J24">
+        <f>$J$19*L6</f>
         <v>291363.21999999997</v>
       </c>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="7" t="s">
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B21">
-        <f>B7*B15</f>
+      <c r="B25">
+        <f>B7*B19</f>
         <v>90169.2</v>
       </c>
-      <c r="C21">
-        <f>$C$15*C7</f>
+      <c r="C25">
+        <f>$C$19*C7</f>
         <v>107153.64</v>
       </c>
-      <c r="D21">
-        <f>$D$15*D7</f>
+      <c r="D25">
+        <f>$D$19*D7</f>
         <v>130895.16</v>
       </c>
-      <c r="E21">
-        <f>$E$15*G7</f>
+      <c r="E25">
+        <f>$E$19*G7</f>
         <v>153829.32749999998</v>
       </c>
-      <c r="F21">
-        <f>$F$15*I7</f>
+      <c r="F25">
+        <f>$F$19*I7</f>
         <v>203374.18</v>
       </c>
-      <c r="G21">
-        <f>$G$15*J7</f>
+      <c r="G25">
+        <f>$G$19*J7</f>
         <v>257350.33</v>
       </c>
-      <c r="H21">
-        <f>$H$15*K7</f>
+      <c r="H25">
+        <f>$H$19*K7</f>
         <v>311326.48</v>
       </c>
-      <c r="I21">
-        <f>$I$15*L7</f>
+      <c r="I25">
+        <f>$I$19*L7</f>
         <v>365302.63</v>
       </c>
-      <c r="J21">
-        <f>$J$15*L7</f>
+      <c r="J25">
+        <f>$J$19*L7</f>
         <v>419278.77999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="27" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="19">
+        <f>B25*$C9</f>
+        <v>35735.258986175111</v>
+      </c>
+      <c r="C26" s="19">
+        <f t="shared" ref="C26:J26" si="0">C25*$C9</f>
+        <v>42466.419539170507</v>
+      </c>
+      <c r="D26" s="19">
+        <f t="shared" si="0"/>
+        <v>51875.501198156686</v>
+      </c>
+      <c r="E26" s="19">
+        <f t="shared" si="0"/>
+        <v>60964.618271889398</v>
+      </c>
+      <c r="F26" s="19">
+        <f t="shared" si="0"/>
+        <v>80599.905437788024</v>
+      </c>
+      <c r="G26" s="19">
+        <f t="shared" si="0"/>
+        <v>101991.37502304147</v>
+      </c>
+      <c r="H26" s="19">
+        <f t="shared" si="0"/>
+        <v>123382.84460829492</v>
+      </c>
+      <c r="I26" s="19">
+        <f t="shared" si="0"/>
+        <v>144774.3141935484</v>
+      </c>
+      <c r="J26" s="19">
+        <f t="shared" si="0"/>
+        <v>166165.78377880182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="19">
+        <f>B25*$C10</f>
+        <v>54433.941013824886</v>
+      </c>
+      <c r="C27" s="19">
+        <f t="shared" ref="C27:J27" si="1">C25*$C10</f>
+        <v>64687.2204608295</v>
+      </c>
+      <c r="D27" s="19">
+        <f t="shared" si="1"/>
+        <v>79019.658801843325</v>
+      </c>
+      <c r="E27" s="19">
+        <f t="shared" si="1"/>
+        <v>92864.709228110602</v>
+      </c>
+      <c r="F27" s="19">
+        <f t="shared" si="1"/>
+        <v>122774.27456221198</v>
+      </c>
+      <c r="G27" s="19">
+        <f t="shared" si="1"/>
+        <v>155358.95497695854</v>
+      </c>
+      <c r="H27" s="19">
+        <f t="shared" si="1"/>
+        <v>187943.63539170509</v>
+      </c>
+      <c r="I27" s="19">
+        <f t="shared" si="1"/>
+        <v>220528.31580645163</v>
+      </c>
+      <c r="J27" s="19">
+        <f t="shared" si="1"/>
+        <v>253112.99622119815</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="27"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="28" t="s">
+      <c r="B29" s="27"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="28"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="7" t="s">
+      <c r="B30" s="28"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="21">
+      <c r="B32" s="21">
         <v>2021</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C32" s="21">
         <v>2022</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D32" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E32" s="7">
         <v>2025</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F32" s="7">
         <v>2030</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G32" s="7">
         <v>2035</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H32" s="7">
         <v>2040</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I32" s="7">
         <v>2045</v>
       </c>
-      <c r="J26" s="7">
+      <c r="J32" s="7">
         <v>2050</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
-      <c r="A27" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>34</v>
       </c>
-      <c r="B27">
+      <c r="B33">
         <v>1159.207116340968</v>
       </c>
-      <c r="C27">
+      <c r="C33">
         <v>1223.8800000000001</v>
       </c>
-      <c r="D27" s="36">
-        <f>AVERAGE(B27:C27)</f>
+      <c r="D33" s="36">
+        <f>AVERAGE(B33:C33)</f>
         <v>1191.5435581704842</v>
       </c>
-      <c r="E27">
-        <f>D27</f>
+      <c r="E33">
+        <f>D33</f>
         <v>1191.5435581704842</v>
       </c>
-      <c r="F27">
-        <f t="shared" ref="F27:J27" si="0">E27</f>
+      <c r="F33">
+        <f t="shared" ref="F33:J33" si="2">E33</f>
         <v>1191.5435581704842</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="0"/>
-        <v>1191.5435581704842</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="0"/>
-        <v>1191.5435581704842</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="0"/>
-        <v>1191.5435581704842</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="0"/>
-        <v>1191.5435581704842</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="26"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="24"/>
-    </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1"/>
-    <row r="31" spans="1:12">
-      <c r="A31" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="14">
-        <v>2020</v>
-      </c>
-      <c r="C31" s="14">
-        <v>2021</v>
-      </c>
-      <c r="D31" s="14">
-        <v>2022</v>
-      </c>
-      <c r="E31" s="14">
-        <v>2025</v>
-      </c>
-      <c r="F31" s="14">
-        <v>2030</v>
-      </c>
-      <c r="G31" s="14">
-        <v>2035</v>
-      </c>
-      <c r="H31" s="14">
-        <v>2040</v>
-      </c>
-      <c r="I31" s="14">
-        <v>2045</v>
-      </c>
-      <c r="J31" s="15">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32">
-        <f>B27*B20</f>
-        <v>53846097.919731043</v>
-      </c>
-      <c r="C32">
-        <f>C20*$D$27</f>
-        <v>65773633.366691671</v>
-      </c>
-      <c r="D32">
-        <f>D20*$D$27</f>
-        <v>80346783.024024621</v>
-      </c>
-      <c r="E32">
-        <f>E20*$D$27</f>
-        <v>118424740.92893277</v>
-      </c>
-      <c r="F32">
-        <f>F20*$D$27</f>
-        <v>168398253.51127768</v>
-      </c>
-      <c r="G32">
-        <f t="shared" ref="G32:J32" si="1">G20*$D$27</f>
-        <v>213091682.10316065</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="1"/>
-        <v>257785110.69504362</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="1"/>
-        <v>302478539.28692663</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="1"/>
-        <v>347171967.87880957</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33">
-        <f>B21*B27</f>
-        <v>104524778.31477201</v>
-      </c>
-      <c r="C33">
-        <f>C21*$D$27</f>
-        <v>127678229.47651912</v>
-      </c>
-      <c r="D33">
-        <f>D21*$D$27</f>
-        <v>155967284.69369483</v>
-      </c>
-      <c r="E33">
-        <f t="shared" ref="E33:J33" si="2">E21*$D$27</f>
-        <v>183294344.24032268</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="2"/>
-        <v>242329194.07720453</v>
       </c>
       <c r="G33">
         <f t="shared" si="2"/>
-        <v>306644127.90454829</v>
+        <v>1191.5435581704842</v>
       </c>
       <c r="H33">
         <f t="shared" si="2"/>
-        <v>370959061.73189205</v>
+        <v>1191.5435581704842</v>
       </c>
       <c r="I33">
         <f t="shared" si="2"/>
-        <v>435273995.55923587</v>
+        <v>1191.5435581704842</v>
       </c>
       <c r="J33">
         <f t="shared" si="2"/>
+        <v>1191.5435581704842</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="26"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="24"/>
+    </row>
+    <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="14">
+        <v>2020</v>
+      </c>
+      <c r="C37" s="14">
+        <v>2021</v>
+      </c>
+      <c r="D37" s="14">
+        <v>2022</v>
+      </c>
+      <c r="E37" s="14">
+        <v>2025</v>
+      </c>
+      <c r="F37" s="14">
+        <v>2030</v>
+      </c>
+      <c r="G37" s="14">
+        <v>2035</v>
+      </c>
+      <c r="H37" s="14">
+        <v>2040</v>
+      </c>
+      <c r="I37" s="14">
+        <v>2045</v>
+      </c>
+      <c r="J37" s="15">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <f>B33*B24</f>
+        <v>53846097.919731043</v>
+      </c>
+      <c r="C38">
+        <f>C24*$D$33</f>
+        <v>65773633.366691671</v>
+      </c>
+      <c r="D38">
+        <f>D24*$D$33</f>
+        <v>80346783.024024621</v>
+      </c>
+      <c r="E38">
+        <f>E24*$D$33</f>
+        <v>118424740.92893277</v>
+      </c>
+      <c r="F38">
+        <f>F24*$D$33</f>
+        <v>168398253.51127768</v>
+      </c>
+      <c r="G38">
+        <f t="shared" ref="G38:J38" si="3">G24*$D$33</f>
+        <v>213091682.10316065</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="3"/>
+        <v>257785110.69504362</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="3"/>
+        <v>302478539.28692663</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="3"/>
+        <v>347171967.87880957</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39">
+        <f>B25*B33</f>
+        <v>104524778.31477201</v>
+      </c>
+      <c r="C39">
+        <f>C25*$D$33</f>
+        <v>127678229.47651912</v>
+      </c>
+      <c r="D39">
+        <f>D25*$D$33</f>
+        <v>155967284.69369483</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ref="E39:J39" si="4">E25*$D$33</f>
+        <v>183294344.24032268</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="4"/>
+        <v>242329194.07720453</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="4"/>
+        <v>306644127.90454829</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="4"/>
+        <v>370959061.73189205</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="4"/>
+        <v>435273995.55923587</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="4"/>
         <v>499588929.38657957</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15" thickBot="1">
-      <c r="A34" s="32" t="s">
+    <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="17">
-        <f>B32+B33</f>
+      <c r="B40" s="17">
+        <f>B38+B39</f>
         <v>158370876.23450306</v>
       </c>
-      <c r="C34" s="17">
-        <f>C32+C33</f>
+      <c r="C40" s="17">
+        <f>C38+C39</f>
         <v>193451862.84321079</v>
       </c>
-      <c r="D34" s="17">
-        <f t="shared" ref="D34:J34" si="3">D32+D33</f>
+      <c r="D40" s="17">
+        <f t="shared" ref="D40:J40" si="5">D38+D39</f>
         <v>236314067.71771944</v>
       </c>
-      <c r="E34" s="17">
-        <f t="shared" si="3"/>
+      <c r="E40" s="17">
+        <f t="shared" si="5"/>
         <v>301719085.16925544</v>
       </c>
-      <c r="F34" s="17">
-        <f t="shared" si="3"/>
+      <c r="F40" s="17">
+        <f t="shared" si="5"/>
         <v>410727447.5884822</v>
       </c>
-      <c r="G34" s="17">
-        <f t="shared" si="3"/>
+      <c r="G40" s="17">
+        <f t="shared" si="5"/>
         <v>519735810.00770891</v>
       </c>
-      <c r="H34" s="17">
-        <f t="shared" si="3"/>
+      <c r="H40" s="17">
+        <f t="shared" si="5"/>
         <v>628744172.42693567</v>
       </c>
-      <c r="I34" s="17">
-        <f t="shared" si="3"/>
+      <c r="I40" s="17">
+        <f t="shared" si="5"/>
         <v>737752534.84616256</v>
       </c>
-      <c r="J34" s="33">
-        <f t="shared" si="3"/>
+      <c r="J40" s="33">
+        <f t="shared" si="5"/>
         <v>846760897.2653892</v>
       </c>
     </row>
@@ -2405,16 +2594,16 @@
   <dimension ref="A1:AF25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
     <col min="2" max="32" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -2512,7 +2701,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -2610,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -2708,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2806,7 +2995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2904,7 +3093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -3002,7 +3191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -3100,136 +3289,136 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" s="41" customFormat="1">
+    <row r="8" spans="1:32" s="41" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>46</v>
       </c>
       <c r="B8" s="41">
-        <f>'Raw data'!B21</f>
-        <v>90169.2</v>
+        <f>'Raw data'!B26</f>
+        <v>35735.258986175111</v>
       </c>
       <c r="C8" s="41">
-        <f>'Raw data'!C21</f>
-        <v>107153.64</v>
+        <f>'Raw data'!C26</f>
+        <v>42466.419539170507</v>
       </c>
       <c r="D8" s="41">
-        <f>'Raw data'!D21</f>
-        <v>130895.16</v>
+        <f>'Raw data'!D26</f>
+        <v>51875.501198156686</v>
       </c>
       <c r="E8" s="41">
         <f>($G$8-$D$8)/($G$1-$D$1)*(E1-$D$1)+$D$8</f>
-        <v>138539.88250000001</v>
+        <v>54905.206889400921</v>
       </c>
       <c r="F8" s="41">
         <f>($G$8-$D$8)/($G$1-$D$1)*(F1-$D$1)+$D$8</f>
-        <v>146184.60499999998</v>
+        <v>57934.912580645163</v>
       </c>
       <c r="G8" s="41">
-        <f>'Raw data'!E21</f>
-        <v>153829.32749999998</v>
+        <f>'Raw data'!E26</f>
+        <v>60964.618271889398</v>
       </c>
       <c r="H8" s="41">
         <f>($L$8-$G$8)/($L$1-$G$1)*(H1-$G$1)+$G$8</f>
-        <v>163738.29799999998</v>
+        <v>64891.675705069123</v>
       </c>
       <c r="I8" s="41">
         <f>($L$8-$G$8)/($L$1-$G$1)*(I1-$G$1)+$G$8</f>
-        <v>173647.26849999998</v>
+        <v>68818.733138248848</v>
       </c>
       <c r="J8" s="41">
         <f>($L$8-$G$8)/($L$1-$G$1)*(J1-$G$1)+$G$8</f>
-        <v>183556.239</v>
+        <v>72745.790571428573</v>
       </c>
       <c r="K8" s="41">
         <f>($L$8-$G$8)/($L$1-$G$1)*(K1-$G$1)+$G$8</f>
-        <v>193465.2095</v>
+        <v>76672.848004608299</v>
       </c>
       <c r="L8" s="41">
-        <f>'Raw data'!F21</f>
-        <v>203374.18</v>
+        <f>'Raw data'!F26</f>
+        <v>80599.905437788024</v>
       </c>
       <c r="M8" s="41">
         <f>($Q$8-$L$8)/($Q$1-$L$1)*(M1-$L$1)+$L$8</f>
-        <v>214169.41</v>
+        <v>84878.199354838711</v>
       </c>
       <c r="N8" s="41">
         <f>($Q$8-$L$8)/($Q$1-$L$1)*(N1-$L$1)+$L$8</f>
-        <v>224964.63999999998</v>
+        <v>89156.493271889398</v>
       </c>
       <c r="O8" s="41">
         <f>($Q$8-$L$8)/($Q$1-$L$1)*(O1-$L$1)+$L$8</f>
-        <v>235759.87</v>
+        <v>93434.787188940099</v>
       </c>
       <c r="P8" s="41">
         <f>($Q$8-$L$8)/($Q$1-$L$1)*(P1-$L$1)+$L$8</f>
-        <v>246555.09999999998</v>
+        <v>97713.081105990786</v>
       </c>
       <c r="Q8" s="41">
-        <f>'Raw data'!G21</f>
-        <v>257350.33</v>
+        <f>'Raw data'!G26</f>
+        <v>101991.37502304147</v>
       </c>
       <c r="R8" s="41">
         <f>($V$8-$Q$8)/($V$1-$Q$1)*(R1-$Q$1)+$Q$8</f>
-        <v>268145.56</v>
+        <v>106269.66894009216</v>
       </c>
       <c r="S8" s="41">
         <f>($V$8-$Q$8)/($V$1-$Q$1)*(S1-$Q$1)+$Q$8</f>
-        <v>278940.78999999998</v>
+        <v>110547.96285714285</v>
       </c>
       <c r="T8" s="41">
         <f>($V$8-$Q$8)/($V$1-$Q$1)*(T1-$Q$1)+$Q$8</f>
-        <v>289736.01999999996</v>
+        <v>114826.25677419355</v>
       </c>
       <c r="U8" s="41">
         <f>($V$8-$Q$8)/($V$1-$Q$1)*(U1-$Q$1)+$Q$8</f>
-        <v>300531.25</v>
+        <v>119104.55069124424</v>
       </c>
       <c r="V8" s="41">
-        <f>'Raw data'!H21</f>
-        <v>311326.48</v>
+        <f>'Raw data'!H26</f>
+        <v>123382.84460829492</v>
       </c>
       <c r="W8" s="41">
         <f>($AA$8-$V$8)/($AA$1-$V$1)*(W1-$V$1)+$V$8</f>
-        <v>322121.70999999996</v>
+        <v>127661.13852534562</v>
       </c>
       <c r="X8" s="41">
         <f>($AA$8-$V$8)/($AA$1-$V$1)*(X1-$V$1)+$V$8</f>
-        <v>332916.94</v>
+        <v>131939.43244239633</v>
       </c>
       <c r="Y8" s="41">
         <f>($AA$8-$V$8)/($AA$1-$V$1)*(Y1-$V$1)+$V$8</f>
-        <v>343712.17</v>
+        <v>136217.726359447</v>
       </c>
       <c r="Z8" s="41">
         <f>($AA$8-$V$8)/($AA$1-$V$1)*(Z1-$V$1)+$V$8</f>
-        <v>354507.4</v>
+        <v>140496.0202764977</v>
       </c>
       <c r="AA8" s="41">
-        <f>'Raw data'!I21</f>
-        <v>365302.63</v>
+        <f>'Raw data'!I26</f>
+        <v>144774.3141935484</v>
       </c>
       <c r="AB8" s="41">
         <f>($AF$8-$AA$8)/($AF$1-$AA$1)*(AB1-$AA$1)+$AA$8</f>
-        <v>376097.86</v>
+        <v>149052.60811059907</v>
       </c>
       <c r="AC8" s="41">
         <f>($AF$8-$AA$8)/($AF$1-$AA$1)*(AC1-$AA$1)+$AA$8</f>
-        <v>386893.08999999997</v>
+        <v>153330.90202764978</v>
       </c>
       <c r="AD8" s="41">
         <f>($AF$8-$AA$8)/($AF$1-$AA$1)*(AD1-$AA$1)+$AA$8</f>
-        <v>397688.32000000001</v>
+        <v>157609.19594470045</v>
       </c>
       <c r="AE8" s="41">
         <f>($AF$8-$AA$8)/($AF$1-$AA$1)*(AE1-$AA$1)+$AA$8</f>
-        <v>408483.55</v>
+        <v>161887.48986175115</v>
       </c>
       <c r="AF8" s="41">
-        <f>'Raw data'!J21</f>
-        <v>419278.77999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32">
+        <f>'Raw data'!J26</f>
+        <v>166165.78377880182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -3327,7 +3516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -3425,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -3523,7 +3712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -3621,7 +3810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -3719,7 +3908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -3817,7 +4006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -3915,7 +4104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -4013,7 +4202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:32">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -4111,7 +4300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -4209,7 +4398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:32">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A19" s="42" t="s">
         <v>57</v>
       </c>
@@ -4307,7 +4496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:32">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A20" s="42" t="s">
         <v>58</v>
       </c>
@@ -4405,7 +4594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:32">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A21" s="42" t="s">
         <v>59</v>
       </c>
@@ -4503,7 +4692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A22" s="42" t="s">
         <v>60</v>
       </c>
@@ -4601,7 +4790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:32">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A23" s="42" t="s">
         <v>61</v>
       </c>
@@ -4699,7 +4888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:32">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A24" s="39" t="s">
         <v>62</v>
       </c>
@@ -4797,7 +4986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:32">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A25" s="39" t="s">
         <v>63</v>
       </c>
@@ -4907,15 +5096,17 @@
   </sheetPr>
   <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="32" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
+    <col min="2" max="32" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -5013,7 +5204,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -5111,7 +5302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -5209,7 +5400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -5307,7 +5498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -5405,7 +5596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -5503,7 +5694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -5601,7 +5792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -5699,7 +5890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -5797,7 +5988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -5895,7 +6086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -5993,7 +6184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -6091,7 +6282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -6189,7 +6380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -6287,7 +6478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -6385,7 +6576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -6483,7 +6674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:32">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -6581,7 +6772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -6679,7 +6870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:32">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A19" s="42" t="s">
         <v>57</v>
       </c>
@@ -6777,7 +6968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:32">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A20" s="42" t="s">
         <v>58</v>
       </c>
@@ -6875,7 +7066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:32">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A21" s="42" t="s">
         <v>59</v>
       </c>
@@ -6973,7 +7164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A22" s="42" t="s">
         <v>60</v>
       </c>
@@ -7071,7 +7262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:32">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A23" s="42" t="s">
         <v>61</v>
       </c>
@@ -7169,7 +7360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:32">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A24" s="39" t="s">
         <v>62</v>
       </c>
@@ -7267,7 +7458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:32">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A25" s="39" t="s">
         <v>63</v>
       </c>
@@ -7377,15 +7568,17 @@
   </sheetPr>
   <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y19" sqref="A14:Y19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="32" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
+    <col min="2" max="32" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -7483,7 +7676,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -7581,7 +7774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -7679,7 +7872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -7777,7 +7970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -7875,7 +8068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -7973,7 +8166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -8071,105 +8264,136 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:32" s="41" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="40">
-        <v>0</v>
-      </c>
-      <c r="C8" s="40">
-        <v>0</v>
-      </c>
-      <c r="D8" s="40">
-        <v>0</v>
-      </c>
-      <c r="E8" s="40">
-        <v>0</v>
-      </c>
-      <c r="F8" s="40">
-        <v>0</v>
-      </c>
-      <c r="G8" s="40">
-        <v>0</v>
-      </c>
-      <c r="H8" s="40">
-        <v>0</v>
-      </c>
-      <c r="I8" s="40">
-        <v>0</v>
-      </c>
-      <c r="J8" s="40">
-        <v>0</v>
-      </c>
-      <c r="K8" s="40">
-        <v>0</v>
-      </c>
-      <c r="L8" s="40">
-        <v>0</v>
-      </c>
-      <c r="M8" s="40">
-        <v>0</v>
-      </c>
-      <c r="N8" s="40">
-        <v>0</v>
-      </c>
-      <c r="O8" s="40">
-        <v>0</v>
-      </c>
-      <c r="P8" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="40">
-        <v>0</v>
-      </c>
-      <c r="R8" s="40">
-        <v>0</v>
-      </c>
-      <c r="S8" s="40">
-        <v>0</v>
-      </c>
-      <c r="T8" s="40">
-        <v>0</v>
-      </c>
-      <c r="U8" s="40">
-        <v>0</v>
-      </c>
-      <c r="V8" s="40">
-        <v>0</v>
-      </c>
-      <c r="W8" s="40">
-        <v>0</v>
-      </c>
-      <c r="X8" s="40">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="40">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="40">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="40">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="40">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="40">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="40">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="40">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32">
+      <c r="B8" s="41">
+        <f>'Raw data'!B27</f>
+        <v>54433.941013824886</v>
+      </c>
+      <c r="C8" s="41">
+        <f>'Raw data'!C27</f>
+        <v>64687.2204608295</v>
+      </c>
+      <c r="D8" s="41">
+        <f>'Raw data'!D27</f>
+        <v>79019.658801843325</v>
+      </c>
+      <c r="E8" s="41">
+        <f>($G$8-$D$8)/($G$1-$D$1)*(E1-$D$1)+$D$8</f>
+        <v>83634.675610599079</v>
+      </c>
+      <c r="F8" s="41">
+        <f>($G$8-$D$8)/($G$1-$D$1)*(F1-$D$1)+$D$8</f>
+        <v>88249.692419354848</v>
+      </c>
+      <c r="G8" s="41">
+        <f>'Raw data'!E27</f>
+        <v>92864.709228110602</v>
+      </c>
+      <c r="H8" s="41">
+        <f>($L$8-$G$8)/($L$1-$G$1)*(H1-$G$1)+$G$8</f>
+        <v>98846.622294930872</v>
+      </c>
+      <c r="I8" s="41">
+        <f>($L$8-$G$8)/($L$1-$G$1)*(I1-$G$1)+$G$8</f>
+        <v>104828.53536175116</v>
+      </c>
+      <c r="J8" s="41">
+        <f>($L$8-$G$8)/($L$1-$G$1)*(J1-$G$1)+$G$8</f>
+        <v>110810.44842857143</v>
+      </c>
+      <c r="K8" s="41">
+        <f>($L$8-$G$8)/($L$1-$G$1)*(K1-$G$1)+$G$8</f>
+        <v>116792.3614953917</v>
+      </c>
+      <c r="L8" s="41">
+        <f>'Raw data'!F27</f>
+        <v>122774.27456221198</v>
+      </c>
+      <c r="M8" s="41">
+        <f>($Q$8-$L$8)/($Q$1-$L$1)*(M1-$L$1)+$L$8</f>
+        <v>129291.21064516129</v>
+      </c>
+      <c r="N8" s="41">
+        <f>($Q$8-$L$8)/($Q$1-$L$1)*(N1-$L$1)+$L$8</f>
+        <v>135808.14672811062</v>
+      </c>
+      <c r="O8" s="41">
+        <f>($Q$8-$L$8)/($Q$1-$L$1)*(O1-$L$1)+$L$8</f>
+        <v>142325.08281105993</v>
+      </c>
+      <c r="P8" s="41">
+        <f>($Q$8-$L$8)/($Q$1-$L$1)*(P1-$L$1)+$L$8</f>
+        <v>148842.01889400923</v>
+      </c>
+      <c r="Q8" s="41">
+        <f>'Raw data'!G27</f>
+        <v>155358.95497695854</v>
+      </c>
+      <c r="R8" s="41">
+        <f>($V$8-$Q$8)/($V$1-$Q$1)*(R1-$Q$1)+$Q$8</f>
+        <v>161875.89105990785</v>
+      </c>
+      <c r="S8" s="41">
+        <f>($V$8-$Q$8)/($V$1-$Q$1)*(S1-$Q$1)+$Q$8</f>
+        <v>168392.82714285716</v>
+      </c>
+      <c r="T8" s="41">
+        <f>($V$8-$Q$8)/($V$1-$Q$1)*(T1-$Q$1)+$Q$8</f>
+        <v>174909.76322580647</v>
+      </c>
+      <c r="U8" s="41">
+        <f>($V$8-$Q$8)/($V$1-$Q$1)*(U1-$Q$1)+$Q$8</f>
+        <v>181426.69930875578</v>
+      </c>
+      <c r="V8" s="41">
+        <f>'Raw data'!H27</f>
+        <v>187943.63539170509</v>
+      </c>
+      <c r="W8" s="41">
+        <f>($AA$8-$V$8)/($AA$1-$V$1)*(W1-$V$1)+$V$8</f>
+        <v>194460.5714746544</v>
+      </c>
+      <c r="X8" s="41">
+        <f>($AA$8-$V$8)/($AA$1-$V$1)*(X1-$V$1)+$V$8</f>
+        <v>200977.50755760371</v>
+      </c>
+      <c r="Y8" s="41">
+        <f>($AA$8-$V$8)/($AA$1-$V$1)*(Y1-$V$1)+$V$8</f>
+        <v>207494.44364055301</v>
+      </c>
+      <c r="Z8" s="41">
+        <f>($AA$8-$V$8)/($AA$1-$V$1)*(Z1-$V$1)+$V$8</f>
+        <v>214011.37972350232</v>
+      </c>
+      <c r="AA8" s="41">
+        <f>'Raw data'!I27</f>
+        <v>220528.31580645163</v>
+      </c>
+      <c r="AB8" s="41">
+        <f>($AF$8-$AA$8)/($AF$1-$AA$1)*(AB1-$AA$1)+$AA$8</f>
+        <v>227045.25188940094</v>
+      </c>
+      <c r="AC8" s="41">
+        <f>($AF$8-$AA$8)/($AF$1-$AA$1)*(AC1-$AA$1)+$AA$8</f>
+        <v>233562.18797235025</v>
+      </c>
+      <c r="AD8" s="41">
+        <f>($AF$8-$AA$8)/($AF$1-$AA$1)*(AD1-$AA$1)+$AA$8</f>
+        <v>240079.12405529956</v>
+      </c>
+      <c r="AE8" s="41">
+        <f>($AF$8-$AA$8)/($AF$1-$AA$1)*(AE1-$AA$1)+$AA$8</f>
+        <v>246596.06013824884</v>
+      </c>
+      <c r="AF8" s="41">
+        <f>'Raw data'!J27</f>
+        <v>253112.99622119815</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -8267,7 +8491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -8365,7 +8589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -8463,7 +8687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -8561,7 +8785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -8659,7 +8883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -8757,7 +8981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -8855,7 +9079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -8953,7 +9177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:32">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -9051,7 +9275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -9149,7 +9373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:32">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A19" s="42" t="s">
         <v>57</v>
       </c>
@@ -9247,7 +9471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:32">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A20" s="42" t="s">
         <v>58</v>
       </c>
@@ -9345,7 +9569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:32">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A21" s="42" t="s">
         <v>59</v>
       </c>
@@ -9443,7 +9667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A22" s="42" t="s">
         <v>60</v>
       </c>
@@ -9541,7 +9765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:32">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A23" s="42" t="s">
         <v>61</v>
       </c>
@@ -9639,7 +9863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:32">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A24" s="39" t="s">
         <v>62</v>
       </c>
@@ -9737,7 +9961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:32">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A25" s="39" t="s">
         <v>63</v>
       </c>
@@ -9841,6 +10065,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -10069,34 +10313,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5B60374-5757-430D-A601-6028B27D7FF5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31BB03D5-F3EE-4A69-A906-27D8CFEDEF51}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64EE33E6-86CE-45F3-86D8-8420B4E5C0AA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64EE33E6-86CE-45F3-86D8-8420B4E5C0AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31BB03D5-F3EE-4A69-A906-27D8CFEDEF51}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5B60374-5757-430D-A601-6028B27D7FF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update MDSC and BDESC
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BDESC/BAU Distributed Electricity Source Capacities.xlsx
+++ b/InputData/bldgs/BDESC/BAU Distributed Electricity Source Capacities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://artelys778.sharepoint.com/sites/Agora-EPStool-Artelys/Documents partages/Artelys/3 - Livrables/1. all data/2. A checker par Paul/Uploaded/10. BAU Distributed Electricity Quantities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\bldgs\BDESC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="8_{C56910BB-A762-4B0B-AC8D-940FC4AECB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3966E3D4-8957-4197-AAFD-CB43D06A4772}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B3CF79-57D1-40CC-B65A-20E600EDDB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" xr2:uid="{018189C1-0CD4-4228-8640-AB6E9BB2D151}"/>
+    <workbookView xWindow="60015" yWindow="3345" windowWidth="23460" windowHeight="13110" activeTab="2" xr2:uid="{018189C1-0CD4-4228-8640-AB6E9BB2D151}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="67">
   <si>
     <t>BDEQ BAU Distributed Electricity Source Capacity</t>
   </si>
@@ -279,6 +279,15 @@
   <si>
     <t>hydrogen combined cycle</t>
   </si>
+  <si>
+    <t>We assume a 50/50 split between commercial and residential rooftop solar.</t>
+  </si>
+  <si>
+    <t>See Solar Power Europe's Figure 11:</t>
+  </si>
+  <si>
+    <t>https://www.solarpowereurope.org/insights/outlooks/eu-market-outlook-for-solar-power-2023-2027/detail</t>
+  </si>
 </sst>
 </file>
 
@@ -288,7 +297,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1301,9 +1310,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1341,7 +1350,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1447,7 +1456,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1589,7 +1598,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1597,28 +1606,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C8B6E5-3AAE-4BB5-A9E2-A69A34ECA6F1}">
-  <dimension ref="B10:D21"/>
+  <dimension ref="B10:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" style="1"/>
+    <col min="1" max="2" width="10.81640625" style="1"/>
     <col min="3" max="3" width="44" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.85546875" style="1"/>
+    <col min="4" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
@@ -1629,7 +1638,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
@@ -1637,7 +1646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
@@ -1645,7 +1654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1653,24 +1662,39 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="38"/>
     </row>
-    <row r="20" spans="2:4" ht="15">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="2:4" ht="15">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C23" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C24" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C25" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1689,37 +1713,37 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
@@ -1757,7 +1781,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1797,7 +1821,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1837,30 +1861,30 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="8"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="9"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="9"/>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1">
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>22</v>
       </c>
@@ -1892,7 +1916,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>23</v>
       </c>
@@ -1924,7 +1948,7 @@
         <v>710642</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>24</v>
       </c>
@@ -1956,7 +1980,7 @@
         <v>2321</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>25</v>
       </c>
@@ -1989,7 +2013,7 @@
         <v>712963</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
         <v>26</v>
       </c>
@@ -2021,7 +2045,7 @@
         <v>85545</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1">
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="16" t="s">
         <v>27</v>
       </c>
@@ -2053,7 +2077,7 @@
         <v>396365</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>28</v>
       </c>
@@ -2096,7 +2120,7 @@
       <c r="K20" s="19"/>
       <c r="L20" s="19"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>29</v>
       </c>
@@ -2137,19 +2161,19 @@
         <v>419278.77999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="27" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="27"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="28"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>32</v>
       </c>
@@ -2181,7 +2205,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2220,20 +2244,20 @@
         <v>1191.5435581704842</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="34" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="26"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="24" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="24"/>
     </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1"/>
-    <row r="31" spans="1:12">
+    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="30" t="s">
         <v>37</v>
       </c>
@@ -2265,7 +2289,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="31" t="s">
         <v>38</v>
       </c>
@@ -2306,7 +2330,7 @@
         <v>347171967.87880957</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="31" t="s">
         <v>29</v>
       </c>
@@ -2347,7 +2371,7 @@
         <v>499588929.38657957</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15" thickBot="1">
+    <row r="34" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="32" t="s">
         <v>23</v>
       </c>
@@ -2404,17 +2428,17 @@
   </sheetPr>
   <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF8" sqref="AF8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
     <col min="2" max="32" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -2512,7 +2536,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -2610,7 +2634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -2708,7 +2732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2806,7 +2830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2904,7 +2928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -3002,7 +3026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -3100,136 +3124,136 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32" s="41" customFormat="1">
+    <row r="8" spans="1:32" s="41" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>46</v>
       </c>
       <c r="B8" s="41">
-        <f>'Raw data'!B21</f>
-        <v>90169.2</v>
+        <f>'Raw data'!B21/2</f>
+        <v>45084.6</v>
       </c>
       <c r="C8" s="41">
-        <f>'Raw data'!C21</f>
-        <v>107153.64</v>
+        <f>'Raw data'!C21/2</f>
+        <v>53576.82</v>
       </c>
       <c r="D8" s="41">
-        <f>'Raw data'!D21</f>
-        <v>130895.16</v>
+        <f>'Raw data'!D21/2</f>
+        <v>65447.58</v>
       </c>
       <c r="E8" s="41">
         <f>($G$8-$D$8)/($G$1-$D$1)*(E1-$D$1)+$D$8</f>
-        <v>138539.88250000001</v>
+        <v>69269.941250000003</v>
       </c>
       <c r="F8" s="41">
         <f>($G$8-$D$8)/($G$1-$D$1)*(F1-$D$1)+$D$8</f>
-        <v>146184.60499999998</v>
+        <v>73092.302499999991</v>
       </c>
       <c r="G8" s="41">
-        <f>'Raw data'!E21</f>
-        <v>153829.32749999998</v>
+        <f>'Raw data'!E21/2</f>
+        <v>76914.663749999992</v>
       </c>
       <c r="H8" s="41">
         <f>($L$8-$G$8)/($L$1-$G$1)*(H1-$G$1)+$G$8</f>
-        <v>163738.29799999998</v>
+        <v>81869.14899999999</v>
       </c>
       <c r="I8" s="41">
         <f>($L$8-$G$8)/($L$1-$G$1)*(I1-$G$1)+$G$8</f>
-        <v>173647.26849999998</v>
+        <v>86823.634249999988</v>
       </c>
       <c r="J8" s="41">
         <f>($L$8-$G$8)/($L$1-$G$1)*(J1-$G$1)+$G$8</f>
-        <v>183556.239</v>
+        <v>91778.119500000001</v>
       </c>
       <c r="K8" s="41">
         <f>($L$8-$G$8)/($L$1-$G$1)*(K1-$G$1)+$G$8</f>
-        <v>193465.2095</v>
+        <v>96732.604749999999</v>
       </c>
       <c r="L8" s="41">
-        <f>'Raw data'!F21</f>
-        <v>203374.18</v>
+        <f>'Raw data'!F21/2</f>
+        <v>101687.09</v>
       </c>
       <c r="M8" s="41">
         <f>($Q$8-$L$8)/($Q$1-$L$1)*(M1-$L$1)+$L$8</f>
-        <v>214169.41</v>
+        <v>107084.705</v>
       </c>
       <c r="N8" s="41">
         <f>($Q$8-$L$8)/($Q$1-$L$1)*(N1-$L$1)+$L$8</f>
-        <v>224964.63999999998</v>
+        <v>112482.31999999999</v>
       </c>
       <c r="O8" s="41">
         <f>($Q$8-$L$8)/($Q$1-$L$1)*(O1-$L$1)+$L$8</f>
-        <v>235759.87</v>
+        <v>117879.935</v>
       </c>
       <c r="P8" s="41">
         <f>($Q$8-$L$8)/($Q$1-$L$1)*(P1-$L$1)+$L$8</f>
-        <v>246555.09999999998</v>
+        <v>123277.54999999999</v>
       </c>
       <c r="Q8" s="41">
-        <f>'Raw data'!G21</f>
-        <v>257350.33</v>
+        <f>'Raw data'!G21/2</f>
+        <v>128675.16499999999</v>
       </c>
       <c r="R8" s="41">
         <f>($V$8-$Q$8)/($V$1-$Q$1)*(R1-$Q$1)+$Q$8</f>
-        <v>268145.56</v>
+        <v>134072.78</v>
       </c>
       <c r="S8" s="41">
         <f>($V$8-$Q$8)/($V$1-$Q$1)*(S1-$Q$1)+$Q$8</f>
-        <v>278940.78999999998</v>
+        <v>139470.39499999999</v>
       </c>
       <c r="T8" s="41">
         <f>($V$8-$Q$8)/($V$1-$Q$1)*(T1-$Q$1)+$Q$8</f>
-        <v>289736.01999999996</v>
+        <v>144868.00999999998</v>
       </c>
       <c r="U8" s="41">
         <f>($V$8-$Q$8)/($V$1-$Q$1)*(U1-$Q$1)+$Q$8</f>
-        <v>300531.25</v>
+        <v>150265.625</v>
       </c>
       <c r="V8" s="41">
-        <f>'Raw data'!H21</f>
-        <v>311326.48</v>
+        <f>'Raw data'!H21/2</f>
+        <v>155663.24</v>
       </c>
       <c r="W8" s="41">
         <f>($AA$8-$V$8)/($AA$1-$V$1)*(W1-$V$1)+$V$8</f>
-        <v>322121.70999999996</v>
+        <v>161060.85499999998</v>
       </c>
       <c r="X8" s="41">
         <f>($AA$8-$V$8)/($AA$1-$V$1)*(X1-$V$1)+$V$8</f>
-        <v>332916.94</v>
+        <v>166458.47</v>
       </c>
       <c r="Y8" s="41">
         <f>($AA$8-$V$8)/($AA$1-$V$1)*(Y1-$V$1)+$V$8</f>
-        <v>343712.17</v>
+        <v>171856.08499999999</v>
       </c>
       <c r="Z8" s="41">
         <f>($AA$8-$V$8)/($AA$1-$V$1)*(Z1-$V$1)+$V$8</f>
-        <v>354507.4</v>
+        <v>177253.7</v>
       </c>
       <c r="AA8" s="41">
-        <f>'Raw data'!I21</f>
-        <v>365302.63</v>
+        <f>'Raw data'!I21/2</f>
+        <v>182651.315</v>
       </c>
       <c r="AB8" s="41">
         <f>($AF$8-$AA$8)/($AF$1-$AA$1)*(AB1-$AA$1)+$AA$8</f>
-        <v>376097.86</v>
+        <v>188048.93</v>
       </c>
       <c r="AC8" s="41">
         <f>($AF$8-$AA$8)/($AF$1-$AA$1)*(AC1-$AA$1)+$AA$8</f>
-        <v>386893.08999999997</v>
+        <v>193446.54499999998</v>
       </c>
       <c r="AD8" s="41">
         <f>($AF$8-$AA$8)/($AF$1-$AA$1)*(AD1-$AA$1)+$AA$8</f>
-        <v>397688.32000000001</v>
+        <v>198844.16</v>
       </c>
       <c r="AE8" s="41">
         <f>($AF$8-$AA$8)/($AF$1-$AA$1)*(AE1-$AA$1)+$AA$8</f>
-        <v>408483.55</v>
+        <v>204241.77499999999</v>
       </c>
       <c r="AF8" s="41">
-        <f>'Raw data'!J21</f>
-        <v>419278.77999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32">
+        <f>'Raw data'!J21/2</f>
+        <v>209639.38999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -3327,7 +3351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -3425,7 +3449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -3523,7 +3547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -3621,7 +3645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -3719,7 +3743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -3817,7 +3841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -3915,7 +3939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -4013,7 +4037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:32">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -4111,7 +4135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -4209,7 +4233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:32">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A19" s="42" t="s">
         <v>57</v>
       </c>
@@ -4307,7 +4331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:32">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A20" s="42" t="s">
         <v>58</v>
       </c>
@@ -4405,7 +4429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:32">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A21" s="42" t="s">
         <v>59</v>
       </c>
@@ -4503,7 +4527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A22" s="42" t="s">
         <v>60</v>
       </c>
@@ -4601,7 +4625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:32">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A23" s="42" t="s">
         <v>61</v>
       </c>
@@ -4699,7 +4723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:32">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A24" s="39" t="s">
         <v>62</v>
       </c>
@@ -4797,7 +4821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:32">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A25" s="39" t="s">
         <v>63</v>
       </c>
@@ -4909,13 +4933,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="32" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
+    <col min="2" max="32" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -5013,7 +5037,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -5111,7 +5135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -5209,7 +5233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -5307,7 +5331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -5405,7 +5429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -5503,7 +5527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -5601,7 +5625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -5699,7 +5723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -5797,7 +5821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -5895,7 +5919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -5993,7 +6017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -6091,7 +6115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -6189,7 +6213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -6287,7 +6311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -6385,7 +6409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -6483,7 +6507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:32">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -6581,7 +6605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -6679,7 +6703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:32">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A19" s="42" t="s">
         <v>57</v>
       </c>
@@ -6777,7 +6801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:32">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A20" s="42" t="s">
         <v>58</v>
       </c>
@@ -6875,7 +6899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:32">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A21" s="42" t="s">
         <v>59</v>
       </c>
@@ -6973,7 +6997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A22" s="42" t="s">
         <v>60</v>
       </c>
@@ -7071,7 +7095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:32">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A23" s="42" t="s">
         <v>61</v>
       </c>
@@ -7169,7 +7193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:32">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A24" s="39" t="s">
         <v>62</v>
       </c>
@@ -7267,7 +7291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:32">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A25" s="39" t="s">
         <v>63</v>
       </c>
@@ -7377,15 +7401,17 @@
   </sheetPr>
   <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:AF8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="32" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
+    <col min="2" max="32" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -7483,7 +7509,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -7581,7 +7607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -7679,7 +7705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -7777,7 +7803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -7875,7 +7901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -7973,7 +7999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -8071,105 +8097,136 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>46</v>
       </c>
       <c r="B8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!B8</f>
+        <v>45084.6</v>
       </c>
       <c r="C8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!C8</f>
+        <v>53576.82</v>
       </c>
       <c r="D8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!D8</f>
+        <v>65447.58</v>
       </c>
       <c r="E8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!E8</f>
+        <v>69269.941250000003</v>
       </c>
       <c r="F8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!F8</f>
+        <v>73092.302499999991</v>
       </c>
       <c r="G8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!G8</f>
+        <v>76914.663749999992</v>
       </c>
       <c r="H8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!H8</f>
+        <v>81869.14899999999</v>
       </c>
       <c r="I8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!I8</f>
+        <v>86823.634249999988</v>
       </c>
       <c r="J8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!J8</f>
+        <v>91778.119500000001</v>
       </c>
       <c r="K8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!K8</f>
+        <v>96732.604749999999</v>
       </c>
       <c r="L8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!L8</f>
+        <v>101687.09</v>
       </c>
       <c r="M8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!M8</f>
+        <v>107084.705</v>
       </c>
       <c r="N8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!N8</f>
+        <v>112482.31999999999</v>
       </c>
       <c r="O8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!O8</f>
+        <v>117879.935</v>
       </c>
       <c r="P8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!P8</f>
+        <v>123277.54999999999</v>
       </c>
       <c r="Q8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!Q8</f>
+        <v>128675.16499999999</v>
       </c>
       <c r="R8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!R8</f>
+        <v>134072.78</v>
       </c>
       <c r="S8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!S8</f>
+        <v>139470.39499999999</v>
       </c>
       <c r="T8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!T8</f>
+        <v>144868.00999999998</v>
       </c>
       <c r="U8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!U8</f>
+        <v>150265.625</v>
       </c>
       <c r="V8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!V8</f>
+        <v>155663.24</v>
       </c>
       <c r="W8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!W8</f>
+        <v>161060.85499999998</v>
       </c>
       <c r="X8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!X8</f>
+        <v>166458.47</v>
       </c>
       <c r="Y8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!Y8</f>
+        <v>171856.08499999999</v>
       </c>
       <c r="Z8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!Z8</f>
+        <v>177253.7</v>
       </c>
       <c r="AA8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!AA8</f>
+        <v>182651.315</v>
       </c>
       <c r="AB8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!AB8</f>
+        <v>188048.93</v>
       </c>
       <c r="AC8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!AC8</f>
+        <v>193446.54499999998</v>
       </c>
       <c r="AD8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!AD8</f>
+        <v>198844.16</v>
       </c>
       <c r="AE8" s="40">
-        <v>0</v>
+        <f>'BDESC-urban-residential'!AE8</f>
+        <v>204241.77499999999</v>
       </c>
       <c r="AF8" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32">
+        <f>'BDESC-urban-residential'!AF8</f>
+        <v>209639.38999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -8267,7 +8324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -8365,7 +8422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -8463,7 +8520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -8561,7 +8618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -8659,7 +8716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -8757,7 +8814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -8855,7 +8912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -8953,7 +9010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:32">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -9051,7 +9108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -9149,7 +9206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:32">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A19" s="42" t="s">
         <v>57</v>
       </c>
@@ -9247,7 +9304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:32">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A20" s="42" t="s">
         <v>58</v>
       </c>
@@ -9345,7 +9402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:32">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A21" s="42" t="s">
         <v>59</v>
       </c>
@@ -9443,7 +9500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A22" s="42" t="s">
         <v>60</v>
       </c>
@@ -9541,7 +9598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:32">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A23" s="42" t="s">
         <v>61</v>
       </c>
@@ -9639,7 +9696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:32">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A24" s="39" t="s">
         <v>62</v>
       </c>
@@ -9737,7 +9794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:32">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A25" s="39" t="s">
         <v>63</v>
       </c>
@@ -9841,6 +9898,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -10069,15 +10135,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -10090,13 +10147,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5B60374-5757-430D-A601-6028B27D7FF5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64EE33E6-86CE-45F3-86D8-8420B4E5C0AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64EE33E6-86CE-45F3-86D8-8420B4E5C0AA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5B60374-5757-430D-A601-6028B27D7FF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31BB03D5-F3EE-4A69-A906-27D8CFEDEF51}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31BB03D5-F3EE-4A69-A906-27D8CFEDEF51}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates rooftop solar lever
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BDESC/BAU Distributed Electricity Source Capacities.xlsx
+++ b/InputData/bldgs/BDESC/BAU Distributed Electricity Source Capacities.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\bldgs\BDESC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B3CF79-57D1-40CC-B65A-20E600EDDB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF32B867-6CFA-4984-A04F-9C8E1584778F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60015" yWindow="3345" windowWidth="23460" windowHeight="13110" activeTab="2" xr2:uid="{018189C1-0CD4-4228-8640-AB6E9BB2D151}"/>
+    <workbookView xWindow="58875" yWindow="510" windowWidth="26355" windowHeight="13470" activeTab="3" xr2:uid="{018189C1-0CD4-4228-8640-AB6E9BB2D151}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Raw data" sheetId="2" r:id="rId2"/>
-    <sheet name="BDESC-urban-residential" sheetId="8" r:id="rId3"/>
-    <sheet name="BDESC-rural-residential" sheetId="9" r:id="rId4"/>
-    <sheet name="BDESC-commercial" sheetId="10" r:id="rId5"/>
+    <sheet name="Ff55 Policy Scenario" sheetId="11" r:id="rId3"/>
+    <sheet name="BDESC-urban-residential" sheetId="8" r:id="rId4"/>
+    <sheet name="BDESC-rural-residential" sheetId="9" r:id="rId5"/>
+    <sheet name="BDESC-commercial" sheetId="10" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="billion_kw_to_MW">#REF!</definedName>
@@ -45,8 +46,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="73">
   <si>
     <t>BDEQ BAU Distributed Electricity Source Capacity</t>
   </si>
@@ -288,16 +311,35 @@
   <si>
     <t>https://www.solarpowereurope.org/insights/outlooks/eu-market-outlook-for-solar-power-2023-2027/detail</t>
   </si>
+  <si>
+    <t>Cumulative installed solar</t>
+  </si>
+  <si>
+    <t>Cumulative installed rooftop solar</t>
+  </si>
+  <si>
+    <t>Share installed</t>
+  </si>
+  <si>
+    <t>https://api.solarpowereurope.org/uploads/SPE_EMO_2023_full_report_c496546963.pdf</t>
+  </si>
+  <si>
+    <t>POLICY SCENARIO:</t>
+  </si>
+  <si>
+    <t>&lt;- POLICY STRINGENCY</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -512,8 +554,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -732,6 +783,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1076,7 +1133,7 @@
     <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1122,6 +1179,11 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="55">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1302,6 +1364,55 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1180646</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>40822</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>450061</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>48416</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{020C490D-0676-4EF3-B07D-D186A069F87C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1180646" y="7984672"/>
+          <a:ext cx="7327565" cy="5900394"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1713,7 +1824,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2422,6 +2533,1072 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7420A5-C3CE-46AA-84A2-AFEF44E59748}">
+  <dimension ref="A1:AF43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" zoomScale="81" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="41.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="25">
+        <v>2020</v>
+      </c>
+      <c r="C5" s="25">
+        <v>2021</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2022</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F5" s="8">
+        <v>2024</v>
+      </c>
+      <c r="G5" s="8">
+        <v>2025</v>
+      </c>
+      <c r="H5" s="5">
+        <v>2026</v>
+      </c>
+      <c r="I5" s="9">
+        <v>2030</v>
+      </c>
+      <c r="J5" s="9">
+        <v>2035</v>
+      </c>
+      <c r="K5" s="9">
+        <v>2040</v>
+      </c>
+      <c r="L5" s="9">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="11">
+        <f>C6</f>
+        <v>0.34</v>
+      </c>
+      <c r="C6" s="11">
+        <f>D6</f>
+        <v>0.34</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.34</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.35750000000000004</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0.39249999999999996</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0.41</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0.41</v>
+      </c>
+      <c r="J6" s="11">
+        <v>0.41</v>
+      </c>
+      <c r="K6" s="11">
+        <v>0.41</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="11">
+        <f>C7</f>
+        <v>0.66</v>
+      </c>
+      <c r="C7" s="11">
+        <f>D7</f>
+        <v>0.66</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.66</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0.64250000000000007</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0.625</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.60749999999999993</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0.59</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0.59</v>
+      </c>
+      <c r="J7" s="11">
+        <v>0.59</v>
+      </c>
+      <c r="K7" s="11">
+        <v>0.59</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="9"/>
+    </row>
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="13">
+        <v>2020</v>
+      </c>
+      <c r="C14" s="13">
+        <v>2021</v>
+      </c>
+      <c r="D14" s="13">
+        <v>2022</v>
+      </c>
+      <c r="E14" s="14">
+        <v>2025</v>
+      </c>
+      <c r="F14" s="14">
+        <v>2030</v>
+      </c>
+      <c r="G14" s="14">
+        <v>2035</v>
+      </c>
+      <c r="H14" s="14">
+        <v>2040</v>
+      </c>
+      <c r="I14" s="14">
+        <v>2045</v>
+      </c>
+      <c r="J14" s="15">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>136620</v>
+      </c>
+      <c r="C15">
+        <v>162354</v>
+      </c>
+      <c r="D15">
+        <v>198326</v>
+      </c>
+      <c r="E15" s="19">
+        <v>253217</v>
+      </c>
+      <c r="F15" s="19">
+        <v>344702</v>
+      </c>
+      <c r="G15" s="19">
+        <v>436187</v>
+      </c>
+      <c r="H15" s="19">
+        <v>527672</v>
+      </c>
+      <c r="I15" s="19">
+        <v>619157</v>
+      </c>
+      <c r="J15" s="20">
+        <v>710642</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>2321</v>
+      </c>
+      <c r="C16">
+        <v>2321</v>
+      </c>
+      <c r="D16">
+        <v>2321</v>
+      </c>
+      <c r="E16">
+        <v>2321</v>
+      </c>
+      <c r="F16">
+        <v>2321</v>
+      </c>
+      <c r="G16">
+        <v>2321</v>
+      </c>
+      <c r="H16">
+        <v>2321</v>
+      </c>
+      <c r="I16">
+        <v>2321</v>
+      </c>
+      <c r="J16" s="29">
+        <v>2321</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <f>B15+B16</f>
+        <v>138941</v>
+      </c>
+      <c r="C17">
+        <v>164675</v>
+      </c>
+      <c r="D17">
+        <v>200647</v>
+      </c>
+      <c r="E17" s="19">
+        <v>255538</v>
+      </c>
+      <c r="F17" s="19">
+        <v>347023</v>
+      </c>
+      <c r="G17" s="19">
+        <v>438508</v>
+      </c>
+      <c r="H17" s="19">
+        <v>529993</v>
+      </c>
+      <c r="I17" s="19">
+        <v>621478</v>
+      </c>
+      <c r="J17" s="20">
+        <v>712963</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>14542</v>
+      </c>
+      <c r="C18">
+        <v>15137</v>
+      </c>
+      <c r="D18">
+        <v>16749</v>
+      </c>
+      <c r="E18" s="19">
+        <v>24120</v>
+      </c>
+      <c r="F18" s="19">
+        <v>36405</v>
+      </c>
+      <c r="G18" s="19">
+        <v>48690</v>
+      </c>
+      <c r="H18" s="19">
+        <v>60975</v>
+      </c>
+      <c r="I18" s="19">
+        <v>73260</v>
+      </c>
+      <c r="J18" s="20">
+        <v>85545</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="17">
+        <v>162590</v>
+      </c>
+      <c r="C19" s="17">
+        <v>173316</v>
+      </c>
+      <c r="D19" s="17">
+        <v>187373</v>
+      </c>
+      <c r="E19" s="22">
+        <v>209765</v>
+      </c>
+      <c r="F19" s="22">
+        <v>247085</v>
+      </c>
+      <c r="G19" s="22">
+        <v>284405</v>
+      </c>
+      <c r="H19" s="22">
+        <v>321725</v>
+      </c>
+      <c r="I19" s="22">
+        <v>359045</v>
+      </c>
+      <c r="J19" s="23">
+        <v>396365</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <f>B15*B6</f>
+        <v>46450.8</v>
+      </c>
+      <c r="C20">
+        <f>$C$15*C6</f>
+        <v>55200.36</v>
+      </c>
+      <c r="D20">
+        <f>$D$15*D6</f>
+        <v>67430.840000000011</v>
+      </c>
+      <c r="E20">
+        <f>$E$15*G6</f>
+        <v>99387.672499999986</v>
+      </c>
+      <c r="F20">
+        <f>$F$15*I6</f>
+        <v>141327.81999999998</v>
+      </c>
+      <c r="G20">
+        <f>$G$15*J6</f>
+        <v>178836.66999999998</v>
+      </c>
+      <c r="H20">
+        <f>$H$15*K6</f>
+        <v>216345.52</v>
+      </c>
+      <c r="I20">
+        <f>$I$15*L6</f>
+        <v>253854.37</v>
+      </c>
+      <c r="J20">
+        <f>$J$15*L6</f>
+        <v>291363.21999999997</v>
+      </c>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <f>B7*B15</f>
+        <v>90169.2</v>
+      </c>
+      <c r="C21">
+        <f>$C$15*C7</f>
+        <v>107153.64</v>
+      </c>
+      <c r="D21">
+        <f>$D$15*D7</f>
+        <v>130895.16</v>
+      </c>
+      <c r="E21">
+        <f>$E$15*G7</f>
+        <v>153829.32749999998</v>
+      </c>
+      <c r="F21">
+        <f>$F$15*I7</f>
+        <v>203374.18</v>
+      </c>
+      <c r="G21">
+        <f>$G$15*J7</f>
+        <v>257350.33</v>
+      </c>
+      <c r="H21">
+        <f>$H$15*K7</f>
+        <v>311326.48</v>
+      </c>
+      <c r="I21">
+        <f>$I$15*L7</f>
+        <v>365302.63</v>
+      </c>
+      <c r="J21">
+        <f>$J$15*L7</f>
+        <v>419278.77999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="27"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="28"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="21">
+        <v>2021</v>
+      </c>
+      <c r="C26" s="21">
+        <v>2022</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="7">
+        <v>2025</v>
+      </c>
+      <c r="F26" s="7">
+        <v>2030</v>
+      </c>
+      <c r="G26" s="7">
+        <v>2035</v>
+      </c>
+      <c r="H26" s="7">
+        <v>2040</v>
+      </c>
+      <c r="I26" s="7">
+        <v>2045</v>
+      </c>
+      <c r="J26" s="7">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>1159.207116340968</v>
+      </c>
+      <c r="C27">
+        <v>1223.8800000000001</v>
+      </c>
+      <c r="D27" s="36">
+        <f>AVERAGE(B27:C27)</f>
+        <v>1191.5435581704842</v>
+      </c>
+      <c r="E27">
+        <f>D27</f>
+        <v>1191.5435581704842</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ref="F27:J27" si="0">E27</f>
+        <v>1191.5435581704842</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>1191.5435581704842</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>1191.5435581704842</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>1191.5435581704842</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>1191.5435581704842</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="26"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="24"/>
+    </row>
+    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="14">
+        <v>2020</v>
+      </c>
+      <c r="C31" s="14">
+        <v>2021</v>
+      </c>
+      <c r="D31" s="14">
+        <v>2022</v>
+      </c>
+      <c r="E31" s="14">
+        <v>2025</v>
+      </c>
+      <c r="F31" s="14">
+        <v>2030</v>
+      </c>
+      <c r="G31" s="14">
+        <v>2035</v>
+      </c>
+      <c r="H31" s="14">
+        <v>2040</v>
+      </c>
+      <c r="I31" s="14">
+        <v>2045</v>
+      </c>
+      <c r="J31" s="15">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32">
+        <f>B27*B20</f>
+        <v>53846097.919731043</v>
+      </c>
+      <c r="C32">
+        <f>C20*$D$27</f>
+        <v>65773633.366691671</v>
+      </c>
+      <c r="D32">
+        <f>D20*$D$27</f>
+        <v>80346783.024024621</v>
+      </c>
+      <c r="E32">
+        <f>E20*$D$27</f>
+        <v>118424740.92893277</v>
+      </c>
+      <c r="F32">
+        <f>F20*$D$27</f>
+        <v>168398253.51127768</v>
+      </c>
+      <c r="G32">
+        <f t="shared" ref="G32:J32" si="1">G20*$D$27</f>
+        <v>213091682.10316065</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>257785110.69504362</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>302478539.28692663</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>347171967.87880957</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A33" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <f>B21*B27</f>
+        <v>104524778.31477201</v>
+      </c>
+      <c r="C33">
+        <f>C21*$D$27</f>
+        <v>127678229.47651912</v>
+      </c>
+      <c r="D33">
+        <f>D21*$D$27</f>
+        <v>155967284.69369483</v>
+      </c>
+      <c r="E33">
+        <f t="shared" ref="E33:J33" si="2">E21*$D$27</f>
+        <v>183294344.24032268</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="2"/>
+        <v>242329194.07720453</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="2"/>
+        <v>306644127.90454829</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="2"/>
+        <v>370959061.73189205</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="2"/>
+        <v>435273995.55923587</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="2"/>
+        <v>499588929.38657957</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="17">
+        <f>B32+B33</f>
+        <v>158370876.23450306</v>
+      </c>
+      <c r="C34" s="17">
+        <f>C32+C33</f>
+        <v>193451862.84321079</v>
+      </c>
+      <c r="D34" s="17">
+        <f t="shared" ref="D34:J34" si="3">D32+D33</f>
+        <v>236314067.71771944</v>
+      </c>
+      <c r="E34" s="17">
+        <f t="shared" si="3"/>
+        <v>301719085.16925544</v>
+      </c>
+      <c r="F34" s="17">
+        <f t="shared" si="3"/>
+        <v>410727447.5884822</v>
+      </c>
+      <c r="G34" s="17">
+        <f t="shared" si="3"/>
+        <v>519735810.00770891</v>
+      </c>
+      <c r="H34" s="17">
+        <f t="shared" si="3"/>
+        <v>628744172.42693567</v>
+      </c>
+      <c r="I34" s="17">
+        <f t="shared" si="3"/>
+        <v>737752534.84616256</v>
+      </c>
+      <c r="J34" s="33">
+        <f t="shared" si="3"/>
+        <v>846760897.2653892</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>2020</v>
+      </c>
+      <c r="C37">
+        <v>2021</v>
+      </c>
+      <c r="D37">
+        <v>2022</v>
+      </c>
+      <c r="E37">
+        <v>2023</v>
+      </c>
+      <c r="F37">
+        <v>2024</v>
+      </c>
+      <c r="G37">
+        <v>2025</v>
+      </c>
+      <c r="H37">
+        <v>2026</v>
+      </c>
+      <c r="I37">
+        <v>2027</v>
+      </c>
+      <c r="J37">
+        <v>2028</v>
+      </c>
+      <c r="K37">
+        <v>2029</v>
+      </c>
+      <c r="L37">
+        <v>2030</v>
+      </c>
+      <c r="M37">
+        <v>2031</v>
+      </c>
+      <c r="N37">
+        <v>2032</v>
+      </c>
+      <c r="O37">
+        <v>2033</v>
+      </c>
+      <c r="P37">
+        <v>2034</v>
+      </c>
+      <c r="Q37">
+        <v>2035</v>
+      </c>
+      <c r="R37">
+        <v>2036</v>
+      </c>
+      <c r="S37">
+        <v>2037</v>
+      </c>
+      <c r="T37">
+        <v>2038</v>
+      </c>
+      <c r="U37">
+        <v>2039</v>
+      </c>
+      <c r="V37">
+        <v>2040</v>
+      </c>
+      <c r="W37">
+        <v>2041</v>
+      </c>
+      <c r="X37">
+        <v>2042</v>
+      </c>
+      <c r="Y37">
+        <v>2043</v>
+      </c>
+      <c r="Z37">
+        <v>2044</v>
+      </c>
+      <c r="AA37">
+        <v>2045</v>
+      </c>
+      <c r="AB37">
+        <v>2046</v>
+      </c>
+      <c r="AC37">
+        <v>2047</v>
+      </c>
+      <c r="AD37">
+        <v>2048</v>
+      </c>
+      <c r="AE37">
+        <v>2049</v>
+      </c>
+      <c r="AF37">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="43">
+        <f>C38/1.2</f>
+        <v>140456.98924731184</v>
+      </c>
+      <c r="C38" s="43">
+        <f>D38/1.24</f>
+        <v>168548.38709677418</v>
+      </c>
+      <c r="D38" s="43">
+        <v>209000</v>
+      </c>
+      <c r="E38" s="43">
+        <v>263000</v>
+      </c>
+      <c r="F38" s="43">
+        <f>E38*1.24</f>
+        <v>326120</v>
+      </c>
+      <c r="G38" s="43">
+        <v>399000</v>
+      </c>
+      <c r="H38" s="44">
+        <f>G38*1.21</f>
+        <v>482790</v>
+      </c>
+      <c r="I38" s="43">
+        <v>576000</v>
+      </c>
+      <c r="L38" s="43">
+        <v>902000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="43">
+        <f>D38*0.66</f>
+        <v>137940</v>
+      </c>
+      <c r="E39" s="43">
+        <v>174000</v>
+      </c>
+      <c r="F39" s="19">
+        <f>F38*F40</f>
+        <v>212068.52430555556</v>
+      </c>
+      <c r="G39" s="19">
+        <f>G38*G40</f>
+        <v>254944.32232256018</v>
+      </c>
+      <c r="H39" s="19">
+        <f>H38*H40</f>
+        <v>303017.74729681556</v>
+      </c>
+      <c r="I39" s="43">
+        <v>355000</v>
+      </c>
+      <c r="J39" s="19">
+        <f>I39+(L39-I39)/3</f>
+        <v>379981.44077418675</v>
+      </c>
+      <c r="K39" s="19">
+        <f>I39+(L39-I39)*2/3</f>
+        <v>404962.88154837344</v>
+      </c>
+      <c r="L39" s="19">
+        <f>175000+G39</f>
+        <v>429944.32232256018</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="10">
+        <f>D39/D38</f>
+        <v>0.66</v>
+      </c>
+      <c r="E40" s="10">
+        <f>E39/E38</f>
+        <v>0.66159695817490494</v>
+      </c>
+      <c r="F40" s="10">
+        <f>$E40+($I40-$E40)*(F37-$E37)/($I37-$E37)</f>
+        <v>0.65027757974228984</v>
+      </c>
+      <c r="G40" s="10">
+        <f>$E40+($I40-$E40)*(G37-$E37)/($I37-$E37)</f>
+        <v>0.63895820130967462</v>
+      </c>
+      <c r="H40" s="10">
+        <f>$E40+($I40-$E40)*(H37-$E37)/($I37-$E37)</f>
+        <v>0.62763882287705952</v>
+      </c>
+      <c r="I40" s="10">
+        <f>I39/I38</f>
+        <v>0.61631944444444442</v>
+      </c>
+      <c r="J40" cm="1">
+        <f t="array" ref="J40">TREND($G40:$I40,$G37:$I37,J37)</f>
+        <v>0.60500006601182932</v>
+      </c>
+      <c r="K40" cm="1">
+        <f t="array" ref="K40">TREND($G40:$I40,$G37:$I37,K37)</f>
+        <v>0.59368068757921222</v>
+      </c>
+      <c r="L40" cm="1">
+        <f t="array" ref="L40">TREND($G40:$I40,$G37:$I37,L37)</f>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="M40">
+        <f>L40</f>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="N40">
+        <f t="shared" ref="N40:AF40" si="4">M40</f>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="Y40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="Z40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="AA40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="AB40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="AC40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="AD40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="AE40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+      <c r="AF40">
+        <f t="shared" si="4"/>
+        <v>0.58236130914659867</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="D41" s="45">
+        <f>D39/MAX($D39:$L39)</f>
+        <v>0.32083223998597726</v>
+      </c>
+      <c r="E41" s="45">
+        <f t="shared" ref="E41:L41" si="5">E39/MAX($D39:$L39)</f>
+        <v>0.40470356501058463</v>
+      </c>
+      <c r="F41" s="45">
+        <f t="shared" si="5"/>
+        <v>0.49324648168386298</v>
+      </c>
+      <c r="G41" s="45">
+        <f t="shared" si="5"/>
+        <v>0.59297055243188324</v>
+      </c>
+      <c r="H41" s="45">
+        <f t="shared" si="5"/>
+        <v>0.70478369306033173</v>
+      </c>
+      <c r="I41" s="45">
+        <f t="shared" si="5"/>
+        <v>0.82568830792389403</v>
+      </c>
+      <c r="J41" s="45">
+        <f t="shared" si="5"/>
+        <v>0.88379220528259606</v>
+      </c>
+      <c r="K41" s="45">
+        <f t="shared" si="5"/>
+        <v>0.94189610264129797</v>
+      </c>
+      <c r="L41" s="45">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A42" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="K42" s="19"/>
+      <c r="L42" s="47">
+        <f>L39/2</f>
+        <v>214972.16116128009</v>
+      </c>
+      <c r="M42" s="46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="L43">
+        <f>L39/L38</f>
+        <v>0.47665667663255007</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="Source : Solar Power europe : Global Market Outlook 2023-2027, figure 21.1" xr:uid="{7BD1DEE4-26E7-4407-BB60-BA114468B471}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1C91AD-8505-4655-9BE0-2634E71F3CC7}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -2429,7 +3606,7 @@
   <dimension ref="A1:AF25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF8" sqref="AF8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4924,7 +6101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4BA7C39-26D7-498E-8FF0-FB7C986760DE}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -7394,7 +8571,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09618D3C-C162-4C12-A357-7A35943E19EA}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -9898,15 +11075,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -10135,7 +11303,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
@@ -10146,15 +11314,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64EE33E6-86CE-45F3-86D8-8420B4E5C0AA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5B60374-5757-430D-A601-6028B27D7FF5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10173,7 +11342,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31BB03D5-F3EE-4A69-A906-27D8CFEDEF51}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -10182,4 +11351,12 @@
     <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64EE33E6-86CE-45F3-86D8-8420B4E5C0AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>